<commit_message>
+2 python scripts almost done; +added possibility to transform test set; +started the report
python scripts and jupyter notebook give consistent results
</commit_message>
<xml_diff>
--- a/out_predictions_v1.xlsx
+++ b/out_predictions_v1.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="out_predictions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -883,7 +883,7 @@
   <dimension ref="A1:K205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>